<commit_message>
Updated README and all affected files
</commit_message>
<xml_diff>
--- a/1-data-collection/experimentation-literature/r3a-venues.xlsx
+++ b/1-data-collection/experimentation-literature/r3a-venues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juf\Workspace\BTH\Data Processing\gere-r3a\1-data-collection\experimentation-literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB8DD62-48CF-4C7F-B7AB-0FCAB346352D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51749A51-C0DD-4498-90EC-2699BCB09B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-14805" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Selection" sheetId="1" r:id="rId1"/>
@@ -814,7 +814,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -825,12 +825,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
         <bgColor rgb="FF666666"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
-        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -908,10 +902,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1147,7 +1141,7 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1519,7 @@
       <c r="E13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>31</v>
       </c>
       <c r="G13" s="5" t="str">
@@ -1554,7 +1548,7 @@
       <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="17" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="5" t="str">
@@ -1960,7 +1954,7 @@
       <c r="E28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="17" t="s">
         <v>60</v>
       </c>
       <c r="G28" s="5" t="str">
@@ -2836,7 +2830,7 @@
       <c r="A36" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>181</v>
       </c>
       <c r="C36" s="7" t="s">
@@ -2913,7 +2907,9 @@
   </sheetPr>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>